<commit_message>
add extra regions and models, turn off defective check
</commit_message>
<xml_diff>
--- a/input_data/available_models_regions_variables_units.xlsx
+++ b/input_data/available_models_regions_variables_units.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gxexakis/Documents/projects/I2AM_PARIS/vetting_process/data_validation_inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gxexakis/Documents/code_archive/i2amparis_validation/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBC7421-3429-FA45-848F-0A0789F3CC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A2C92D-383F-B249-821C-FAA1B5BB12BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6440" yWindow="-21040" windowWidth="28800" windowHeight="17500" tabRatio="804" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" tabRatio="804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variable_units" sheetId="13" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3942" uniqueCount="2201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3999" uniqueCount="2231">
   <si>
     <t>Variable</t>
   </si>
@@ -6669,6 +6669,96 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>GEMINI-E3 8.0</t>
+  </si>
+  <si>
+    <t>GEMINI-E3 7.0</t>
+  </si>
+  <si>
+    <t>DEU</t>
+  </si>
+  <si>
+    <t>FRA</t>
+  </si>
+  <si>
+    <t>ITA</t>
+  </si>
+  <si>
+    <t>SPN</t>
+  </si>
+  <si>
+    <t>NLD</t>
+  </si>
+  <si>
+    <t>SWE</t>
+  </si>
+  <si>
+    <t>POL</t>
+  </si>
+  <si>
+    <t>BEL</t>
+  </si>
+  <si>
+    <t>EU1</t>
+  </si>
+  <si>
+    <t>EU2</t>
+  </si>
+  <si>
+    <t>EU3</t>
+  </si>
+  <si>
+    <t>EU4</t>
+  </si>
+  <si>
+    <t>EU5</t>
+  </si>
+  <si>
+    <t>EU6</t>
+  </si>
+  <si>
+    <t>GBR</t>
+  </si>
+  <si>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>RUS</t>
+  </si>
+  <si>
+    <t>CSA</t>
+  </si>
+  <si>
+    <t>MID</t>
+  </si>
+  <si>
+    <t>AFR</t>
+  </si>
+  <si>
+    <t>ASI</t>
+  </si>
+  <si>
+    <t>ROW</t>
+  </si>
+  <si>
+    <t>WORLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">billion US$2010/yr or local currency/yr </t>
+  </si>
+  <si>
+    <t>billion US$2010/yr OR local currency</t>
+  </si>
+  <si>
+    <t>US$2010/GJ or local currency/GJ</t>
+  </si>
+  <si>
+    <t>billion US$2010/yr or local currency/yr</t>
   </si>
 </sst>
 </file>
@@ -6797,9 +6887,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6837,9 +6927,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6872,26 +6962,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6924,26 +6997,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7120,10 +7176,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:B1814"/>
+  <dimension ref="A1:B1829"/>
   <sheetViews>
-    <sheetView topLeftCell="A1918" workbookViewId="0">
-      <selection activeCell="A386" sqref="A386"/>
+    <sheetView tabSelected="1" topLeftCell="A1783" workbookViewId="0">
+      <selection activeCell="A1830" sqref="A1830:B1835"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21644,13 +21700,133 @@
         <v>1606</v>
       </c>
     </row>
+    <row r="1815" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1815" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1815" t="s">
+        <v>2227</v>
+      </c>
+    </row>
+    <row r="1816" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1816" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1816" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="1817" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1817" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1817" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="1818" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1818" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B1818" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="1819" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1819" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1819" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="1820" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1820" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1820" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="1821" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1821" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1821" s="2" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="1822" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1822" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1822" s="2" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="1823" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1823" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1823" s="2" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="1824" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1824" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B1824" s="2" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="1825" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1825" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B1825" t="s">
+        <v>2230</v>
+      </c>
+    </row>
+    <row r="1826" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1826" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1826" t="s">
+        <v>2229</v>
+      </c>
+    </row>
+    <row r="1827" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1827" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1827" s="2" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="1828" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1828" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1828" s="2" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="1829" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1829" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1829" s="2" t="s">
+        <v>2228</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{63CBDA78-E778-48B9-8708-3A0D83BE0464}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B1812">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A2:A1814">
+  <conditionalFormatting sqref="A2:A1831">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21659,10 +21835,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EC4F10-1622-264E-8E9E-AAD4F9058A0A}">
-  <dimension ref="A1:A50"/>
+  <dimension ref="A1:A52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21917,6 +22093,16 @@
         <v>1939</v>
       </c>
     </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>2201</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>2202</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21924,10 +22110,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42F6456-7873-3F47-94D9-95BCFC74D9F5}">
-  <dimension ref="A1:A265"/>
+  <dimension ref="A1:A290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
-      <selection activeCell="D237" sqref="D237"/>
+    <sheetView topLeftCell="A246" workbookViewId="0">
+      <selection activeCell="D273" sqref="D273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23255,6 +23441,131 @@
     <row r="265" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>2182</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>2203</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>2204</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>2205</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>2206</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>2207</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>2208</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>2209</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>2210</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>2211</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
+        <v>2213</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
+        <v>2214</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>2215</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>2216</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
+        <v>2217</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
+        <v>2218</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
+        <v>2219</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A284" t="s">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A285" t="s">
+        <v>2221</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>2222</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A287" t="s">
+        <v>2223</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A288" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A289" t="s">
+        <v>2225</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
+        <v>2226</v>
       </c>
     </row>
   </sheetData>
@@ -23268,15 +23579,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CA09B611E82E044D956B04788434B279" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="63db924393ce496d7b3c7e8d0fe88ab4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="947e1231-797c-4c4e-88f0-3c2d77cf6589" xmlns:ns3="2ac8e7bc-b8df-4926-831d-c1fd22c8bc48" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dd27cc0c36bdcd4e953137e07af95417" ns2:_="" ns3:_="">
     <xsd:import namespace="947e1231-797c-4c4e-88f0-3c2d77cf6589"/>
@@ -23493,6 +23795,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -23500,14 +23811,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D337DC73-A9B2-4807-BE09-B2344465A4BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A2C8DE5-E266-4F50-B68B-8C4D1AA09AD0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23522,6 +23825,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D337DC73-A9B2-4807-BE09-B2344465A4BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>